<commit_message>
sr_ctr_xl qls, other qls, fix template tasks/d90057c4-7518-4a8d-b9da-7ec7408faf0f
</commit_message>
<xml_diff>
--- a/mosgis-web/src/main/webapp/_/libs/mosgis/Шаблон_импорта_сведений_о_договорах_ресурсоснабжения.xlsx
+++ b/mosgis-web/src/main/webapp/_/libs/mosgis/Шаблон_импорта_сведений_о_договорах_ресурсоснабжения.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\mosgis\mosgis-web\src\main\webapp\_\libs\mosgis\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57484233-A426-44D0-8336-1391600DE11A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19080" yWindow="-120" windowWidth="28110" windowHeight="16440" tabRatio="654" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="654" firstSheet="4" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Договоры ресурсоснабжения" sheetId="1" r:id="rId1"/>
@@ -28,6 +22,7 @@
     <sheet name="Справочник КР" sheetId="11" state="hidden" r:id="rId13"/>
     <sheet name="Справочник показателей качества" sheetId="12" state="hidden" r:id="rId14"/>
     <sheet name="Справочник оснований заключения" sheetId="15" state="hidden" r:id="rId15"/>
+    <sheet name="Тип Поля" sheetId="29" state="hidden" r:id="rId16"/>
   </sheets>
   <definedNames>
     <definedName name="Адрес_ОЖФ">'Объекты жилищного фонда'!$C$2:$C$1048576</definedName>
@@ -67,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="167">
   <si>
     <t>Номер договора</t>
   </si>
@@ -339,66 +334,129 @@
     <t>Паспорт гражданина Российской Федерации</t>
   </si>
   <si>
+    <t>1          </t>
+  </si>
+  <si>
     <t>Паспорт гражданина СССР</t>
   </si>
   <si>
+    <t>2          </t>
+  </si>
+  <si>
     <t>Паспорт гражданина иностранного государства</t>
   </si>
   <si>
+    <t>3          </t>
+  </si>
+  <si>
     <t>Общегражданский заграничный паспорт</t>
   </si>
   <si>
+    <t>4          </t>
+  </si>
+  <si>
     <t>Заграничный паспорт Министерства морского флота</t>
   </si>
   <si>
+    <t>5          </t>
+  </si>
+  <si>
     <t>Дипломатический паспорт</t>
   </si>
   <si>
+    <t>6          </t>
+  </si>
+  <si>
     <t>Паспорт моряка (удостоверение личности моряка)</t>
   </si>
   <si>
+    <t>7          </t>
+  </si>
+  <si>
     <t>Военный билет военнослужащего</t>
   </si>
   <si>
+    <t>8          </t>
+  </si>
+  <si>
     <t>Временное удостоверение, выданное взамен военного билета</t>
   </si>
   <si>
+    <t>9          </t>
+  </si>
+  <si>
     <t>Удостоверение личности офицера Министерства обороны Российской Федерации, Министерства внутренних дел Российской Федерации и других воинских формирований с приложением справки о прописке (регистрации) Ф-33</t>
   </si>
   <si>
+    <t>10      </t>
+  </si>
+  <si>
     <t>Свидетельство о рождении</t>
   </si>
   <si>
+    <t>11      </t>
+  </si>
+  <si>
     <t>Свидетельство о рассмотрении ходатайства о признании беженцем на территории Российской Федерации по существу</t>
   </si>
   <si>
+    <t>12      </t>
+  </si>
+  <si>
     <t>Вид на жительство иностранного гражданина или лица без гражданства</t>
   </si>
   <si>
+    <t>13      </t>
+  </si>
+  <si>
     <t>Справка об освобождении из мест лишения свободы</t>
   </si>
   <si>
+    <t>14      </t>
+  </si>
+  <si>
     <t>Временное удостоверение личности гражданина Российской Федерации</t>
   </si>
   <si>
+    <t>15      </t>
+  </si>
+  <si>
     <t>Удостоверение вынужденного переселенца</t>
   </si>
   <si>
+    <t>16      </t>
+  </si>
+  <si>
     <t>Разрешение на временное проживание в Российской Федерации</t>
   </si>
   <si>
+    <t>17      </t>
+  </si>
+  <si>
     <t>Удостоверение беженца в Российской Федерации</t>
   </si>
   <si>
+    <t>18      </t>
+  </si>
+  <si>
     <t>Свидетельство о рассмотрении ходатайства о признании лица вынужденным переселенцем</t>
   </si>
   <si>
+    <t>19      </t>
+  </si>
+  <si>
     <t>Свидетельство о предоставлении временного убежища на территории Российской Федерации</t>
   </si>
   <si>
+    <t>20      </t>
+  </si>
+  <si>
     <t>Иные документы, предусмотренные законодательством Российской Федерации или признаваемые в соответствии с международным договором Российской Федерации в качестве документов, удостоверяющих личность</t>
   </si>
   <si>
+    <t>21      </t>
+  </si>
+  <si>
     <t>Загранпаспорт гражданина бывшего СССР</t>
   </si>
   <si>
@@ -483,9 +541,6 @@
     <t>Порядок размещения информации о начислениях за коммунальные услуги ведется</t>
   </si>
   <si>
-    <t>Размещение информации  о начислениях за коммунальные услуги осуществляет</t>
-  </si>
-  <si>
     <t>UNOM</t>
   </si>
   <si>
@@ -505,12 +560,24 @@
   </si>
   <si>
     <t>Общая площадь помещения (комнаты)</t>
+  </si>
+  <si>
+    <t>Тип Поля</t>
+  </si>
+  <si>
+    <t>Число</t>
+  </si>
+  <si>
+    <t>Логическое</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Тип показателя </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="000000"/>
     <numFmt numFmtId="165" formatCode="#,##0.0000"/>
@@ -705,7 +772,7 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -802,46 +869,46 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="5" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="6" borderId="1" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="5" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="3" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="6" borderId="3" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="7" fillId="6" borderId="2" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="6" borderId="3" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="6" fillId="5" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="6" borderId="1" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -850,27 +917,30 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="5" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="164" fontId="7" fillId="6" borderId="4" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="6" borderId="5" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="5" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="6" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="6" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -883,9 +953,10 @@
     <xf numFmtId="14" fontId="7" fillId="6" borderId="1" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
-    <cellStyle name="40% — акцент1" xfId="3" builtinId="31"/>
+    <cellStyle name="40% - Акцент1" xfId="3" builtinId="31"/>
     <cellStyle name="Нейтральный" xfId="2" builtinId="28"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
     <cellStyle name="Хороший" xfId="1" builtinId="26"/>
@@ -1158,19 +1229,19 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AP2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A3" sqref="A3"/>
+      <selection pane="topRight" activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1219,11 +1290,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:42" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="36" t="s">
-        <v>115</v>
-      </c>
-      <c r="B1" s="46" t="s">
-        <v>137</v>
+      <c r="A1" s="54" t="s">
+        <v>136</v>
+      </c>
+      <c r="B1" s="37" t="s">
+        <v>157</v>
       </c>
       <c r="C1" s="50" t="s">
         <v>0</v>
@@ -1231,152 +1302,152 @@
       <c r="D1" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="41" t="s">
+      <c r="E1" s="52" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="42" t="s">
+      <c r="F1" s="56" t="s">
+        <v>152</v>
+      </c>
+      <c r="G1" s="47" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="37" t="s">
+        <v>158</v>
+      </c>
+      <c r="I1" s="55" t="s">
+        <v>29</v>
+      </c>
+      <c r="J1" s="49" t="s">
+        <v>65</v>
+      </c>
+      <c r="K1" s="49" t="s">
+        <v>66</v>
+      </c>
+      <c r="L1" s="49" t="s">
+        <v>67</v>
+      </c>
+      <c r="M1" s="56" t="s">
+        <v>68</v>
+      </c>
+      <c r="N1" s="47" t="s">
+        <v>69</v>
+      </c>
+      <c r="O1" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="P1" s="48" t="s">
+        <v>129</v>
+      </c>
+      <c r="Q1" s="48" t="s">
+        <v>130</v>
+      </c>
+      <c r="R1" s="48" t="s">
         <v>131</v>
       </c>
-      <c r="G1" s="44" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1" s="46" t="s">
-        <v>138</v>
-      </c>
-      <c r="I1" s="37" t="s">
-        <v>29</v>
-      </c>
-      <c r="J1" s="45" t="s">
-        <v>65</v>
-      </c>
-      <c r="K1" s="45" t="s">
-        <v>66</v>
-      </c>
-      <c r="L1" s="45" t="s">
-        <v>67</v>
-      </c>
-      <c r="M1" s="42" t="s">
-        <v>68</v>
-      </c>
-      <c r="N1" s="44" t="s">
-        <v>69</v>
-      </c>
-      <c r="O1" s="39" t="s">
-        <v>70</v>
-      </c>
-      <c r="P1" s="39" t="s">
-        <v>108</v>
-      </c>
-      <c r="Q1" s="39" t="s">
-        <v>109</v>
-      </c>
-      <c r="R1" s="39" t="s">
-        <v>110</v>
-      </c>
-      <c r="S1" s="39" t="s">
-        <v>111</v>
-      </c>
-      <c r="T1" s="49" t="s">
+      <c r="S1" s="48" t="s">
+        <v>132</v>
+      </c>
+      <c r="T1" s="39" t="s">
         <v>62</v>
       </c>
-      <c r="U1" s="49" t="s">
+      <c r="U1" s="39" t="s">
         <v>63</v>
       </c>
-      <c r="V1" s="49" t="s">
+      <c r="V1" s="39" t="s">
         <v>64</v>
       </c>
-      <c r="W1" s="58" t="s">
-        <v>129</v>
-      </c>
-      <c r="X1" s="55" t="s">
-        <v>112</v>
-      </c>
-      <c r="Y1" s="56"/>
-      <c r="Z1" s="53" t="s">
+      <c r="W1" s="44" t="s">
+        <v>150</v>
+      </c>
+      <c r="X1" s="40" t="s">
+        <v>133</v>
+      </c>
+      <c r="Y1" s="41"/>
+      <c r="Z1" s="58" t="s">
         <v>60</v>
       </c>
-      <c r="AA1" s="54"/>
-      <c r="AB1" s="55" t="s">
+      <c r="AA1" s="59"/>
+      <c r="AB1" s="40" t="s">
         <v>80</v>
       </c>
-      <c r="AC1" s="56"/>
-      <c r="AD1" s="57" t="s">
-        <v>130</v>
-      </c>
-      <c r="AE1" s="48" t="s">
-        <v>127</v>
-      </c>
-      <c r="AF1" s="44"/>
-      <c r="AG1" s="44"/>
-      <c r="AH1" s="44"/>
-      <c r="AI1" s="41" t="s">
+      <c r="AC1" s="41"/>
+      <c r="AD1" s="42" t="s">
+        <v>151</v>
+      </c>
+      <c r="AE1" s="46" t="s">
+        <v>148</v>
+      </c>
+      <c r="AF1" s="47"/>
+      <c r="AG1" s="47"/>
+      <c r="AH1" s="47"/>
+      <c r="AI1" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="AJ1" s="57" t="s">
-        <v>134</v>
-      </c>
-      <c r="AK1" s="48" t="s">
-        <v>125</v>
-      </c>
-      <c r="AL1" s="57" t="s">
-        <v>126</v>
-      </c>
-      <c r="AM1" s="46" t="s">
+      <c r="AJ1" s="42" t="s">
+        <v>155</v>
+      </c>
+      <c r="AK1" s="46" t="s">
+        <v>146</v>
+      </c>
+      <c r="AL1" s="42" t="s">
+        <v>147</v>
+      </c>
+      <c r="AM1" s="37" t="s">
         <v>85</v>
       </c>
-      <c r="AN1" s="46" t="s">
+      <c r="AN1" s="37" t="s">
         <v>61</v>
       </c>
-      <c r="AO1" s="52" t="s">
-        <v>132</v>
-      </c>
-      <c r="AP1" s="39" t="s">
+      <c r="AO1" s="53" t="s">
+        <v>153</v>
+      </c>
+      <c r="AP1" s="48" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:42" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="36"/>
-      <c r="B2" s="47"/>
+      <c r="A2" s="54"/>
+      <c r="B2" s="38"/>
       <c r="C2" s="50"/>
       <c r="D2" s="51"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="47"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="45"/>
-      <c r="K2" s="45"/>
-      <c r="L2" s="45"/>
-      <c r="M2" s="43"/>
-      <c r="N2" s="44"/>
-      <c r="O2" s="40"/>
-      <c r="P2" s="40"/>
-      <c r="Q2" s="40"/>
-      <c r="R2" s="40"/>
-      <c r="S2" s="40"/>
-      <c r="T2" s="49"/>
-      <c r="U2" s="49"/>
-      <c r="V2" s="49"/>
-      <c r="W2" s="40"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="57"/>
+      <c r="G2" s="47"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="43"/>
+      <c r="J2" s="49"/>
+      <c r="K2" s="49"/>
+      <c r="L2" s="49"/>
+      <c r="M2" s="57"/>
+      <c r="N2" s="47"/>
+      <c r="O2" s="45"/>
+      <c r="P2" s="45"/>
+      <c r="Q2" s="45"/>
+      <c r="R2" s="45"/>
+      <c r="S2" s="45"/>
+      <c r="T2" s="39"/>
+      <c r="U2" s="39"/>
+      <c r="V2" s="39"/>
+      <c r="W2" s="45"/>
       <c r="X2" s="31" t="s">
-        <v>114</v>
+        <v>135</v>
       </c>
       <c r="Y2" s="31" t="s">
-        <v>113</v>
+        <v>134</v>
       </c>
       <c r="Z2" s="31" t="s">
-        <v>114</v>
+        <v>135</v>
       </c>
       <c r="AA2" s="31" t="s">
-        <v>113</v>
+        <v>134</v>
       </c>
       <c r="AB2" s="31" t="s">
-        <v>114</v>
+        <v>135</v>
       </c>
       <c r="AC2" s="31" t="s">
-        <v>113</v>
-      </c>
-      <c r="AD2" s="38"/>
+        <v>134</v>
+      </c>
+      <c r="AD2" s="43"/>
       <c r="AE2" s="31" t="s">
         <v>4</v>
       </c>
@@ -1389,26 +1460,28 @@
       <c r="AH2" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="AI2" s="41"/>
-      <c r="AJ2" s="38"/>
-      <c r="AK2" s="44"/>
-      <c r="AL2" s="38"/>
-      <c r="AM2" s="47"/>
-      <c r="AN2" s="47"/>
-      <c r="AO2" s="52"/>
-      <c r="AP2" s="40"/>
+      <c r="AI2" s="52"/>
+      <c r="AJ2" s="43"/>
+      <c r="AK2" s="47"/>
+      <c r="AL2" s="43"/>
+      <c r="AM2" s="38"/>
+      <c r="AN2" s="38"/>
+      <c r="AO2" s="53"/>
+      <c r="AP2" s="45"/>
     </row>
   </sheetData>
   <mergeCells count="36">
-    <mergeCell ref="AM1:AM2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="V1:V2"/>
-    <mergeCell ref="X1:Y1"/>
-    <mergeCell ref="AL1:AL2"/>
-    <mergeCell ref="W1:W2"/>
-    <mergeCell ref="AD1:AD2"/>
-    <mergeCell ref="AJ1:AJ2"/>
-    <mergeCell ref="AK1:AK2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="O1:O2"/>
+    <mergeCell ref="AI1:AI2"/>
+    <mergeCell ref="M1:M2"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="J1:J2"/>
+    <mergeCell ref="K1:K2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="Z1:AA1"/>
+    <mergeCell ref="AB1:AC1"/>
     <mergeCell ref="AP1:AP2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="B1:B2"/>
@@ -1425,58 +1498,56 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="E1:E2"/>
     <mergeCell ref="AO1:AO2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="O1:O2"/>
-    <mergeCell ref="AI1:AI2"/>
-    <mergeCell ref="M1:M2"/>
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="J1:J2"/>
-    <mergeCell ref="K1:K2"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="Z1:AA1"/>
-    <mergeCell ref="AB1:AC1"/>
+    <mergeCell ref="AM1:AM2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="V1:V2"/>
+    <mergeCell ref="X1:Y1"/>
+    <mergeCell ref="AL1:AL2"/>
+    <mergeCell ref="W1:W2"/>
+    <mergeCell ref="AD1:AD2"/>
+    <mergeCell ref="AJ1:AJ2"/>
+    <mergeCell ref="AK1:AK2"/>
   </mergeCells>
   <dataValidations count="13">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AK3:AK1048576" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AK3:AK1048576">
       <formula1>"РСО, Исполнитель коммунальных услуг"</formula1>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AG3:AG1048576 Z3:Z1048576 AB3:AB1048576 X4:X1048576" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AG3:AG1048576 Z3:Z1048576 AB3:AB1048576 X4:X1048576">
       <formula1>-1</formula1>
       <formula2>30</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AF3:AF1048576" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AF3:AF1048576">
       <formula1>"Да,Нет"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AH3:AH1048576 B3:B1048576 AN3:AN1048576" xr:uid="{00000000-0002-0000-0000-000003000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AH3:AH1048576 B3:B1048576 AN3:AN1048576">
       <formula1>"Да, Нет"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I3:I1048576" xr:uid="{00000000-0002-0000-0000-000004000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I3:I1048576">
       <formula1>"Физическое лицо, Юридическое лицо, Индивидуальный предприниматель, Не указывать собственника/пользователя"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M3:M1048576" xr:uid="{00000000-0002-0000-0000-000005000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M3:M1048576">
       <formula1>"м, ж"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AI3:AI1048576" xr:uid="{00000000-0002-0000-0000-000006000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AI3:AI1048576">
       <formula1>Основания_заключения</formula1>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AE3:AE1048576" xr:uid="{00000000-0002-0000-0000-000007000000}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AE3:AE1048576">
       <formula1>1</formula1>
       <formula2>30</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H3:H1048576" xr:uid="{00000000-0002-0000-0000-000008000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H3:H1048576">
       <formula1>"Собственник или пользователь жилого (нежилого) помещения в МКД, Собственник или пользователь жилого дома (домовладения), Управляющая организация, Договор оферта, Представитель собственников МКД, Единоличный собственник помещений в МКД"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AM3:AM1048576 AJ3:AJ1048576 AO3:AO1048576" xr:uid="{00000000-0002-0000-0000-000009000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AM3:AM1048576 AJ3:AJ1048576 AO3:AO1048576">
       <formula1>"В разрезе договора, В разрезе ОЖФ"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P3:P1048576" xr:uid="{00000000-0002-0000-0000-00000A000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P3:P1048576">
       <formula1>Виды_документов</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Y3:Y1048576 AA3:AA1048576 AC3:AC1048576" xr:uid="{00000000-0002-0000-0000-00000B000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Y3:Y1048576 AA3:AA1048576 AC3:AC1048576">
       <formula1>"текущего расчетного месяца, следующего месяца за расчетным"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AL3:AL1048576 W3:W1048576 AD3:AD1048576 F3:F1048576" xr:uid="{00000000-0002-0000-0000-00000C000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AL3:AL1048576 W3:W1048576 AD3:AD1048576 F3:F1048576">
       <formula1>Признак</formula1>
     </dataValidation>
   </dataValidations>
@@ -1486,7 +1557,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1495,12 +1566,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>118</v>
+        <v>139</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>119</v>
+        <v>140</v>
       </c>
     </row>
   </sheetData>
@@ -1509,11 +1580,11 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1525,173 +1596,173 @@
       <c r="A1" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="B1" s="26">
-        <v>1</v>
+      <c r="B1" s="26" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>87</v>
-      </c>
-      <c r="B2" s="26">
-        <v>2</v>
+        <v>88</v>
+      </c>
+      <c r="B2" s="26" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
-        <v>88</v>
-      </c>
-      <c r="B3" s="26">
-        <v>3</v>
+        <v>90</v>
+      </c>
+      <c r="B3" s="26" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
-        <v>89</v>
-      </c>
-      <c r="B4" s="26">
-        <v>4</v>
+        <v>92</v>
+      </c>
+      <c r="B4" s="26" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="B5" s="26">
-        <v>5</v>
+        <v>94</v>
+      </c>
+      <c r="B5" s="26" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
-        <v>91</v>
-      </c>
-      <c r="B6" s="26">
-        <v>6</v>
+        <v>96</v>
+      </c>
+      <c r="B6" s="26" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
-        <v>92</v>
-      </c>
-      <c r="B7" s="26">
-        <v>7</v>
+        <v>98</v>
+      </c>
+      <c r="B7" s="26" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
-        <v>93</v>
-      </c>
-      <c r="B8" s="26">
-        <v>8</v>
+        <v>100</v>
+      </c>
+      <c r="B8" s="26" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="B9" s="26">
-        <v>9</v>
+        <v>102</v>
+      </c>
+      <c r="B9" s="26" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="B10" s="26">
-        <v>10</v>
+        <v>104</v>
+      </c>
+      <c r="B10" s="26" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
-        <v>96</v>
-      </c>
-      <c r="B11" s="26">
-        <v>11</v>
+        <v>106</v>
+      </c>
+      <c r="B11" s="26" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
-        <v>97</v>
-      </c>
-      <c r="B12" s="26">
-        <v>12</v>
+        <v>108</v>
+      </c>
+      <c r="B12" s="26" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
-        <v>98</v>
-      </c>
-      <c r="B13" s="26">
-        <v>13</v>
+        <v>110</v>
+      </c>
+      <c r="B13" s="26" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
-        <v>99</v>
-      </c>
-      <c r="B14" s="26">
-        <v>14</v>
+        <v>112</v>
+      </c>
+      <c r="B14" s="26" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
-        <v>100</v>
-      </c>
-      <c r="B15" s="26">
-        <v>15</v>
+        <v>114</v>
+      </c>
+      <c r="B15" s="26" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
-        <v>101</v>
-      </c>
-      <c r="B16" s="26">
-        <v>16</v>
+        <v>116</v>
+      </c>
+      <c r="B16" s="26" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
-        <v>102</v>
-      </c>
-      <c r="B17" s="26">
-        <v>17</v>
+        <v>118</v>
+      </c>
+      <c r="B17" s="26" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="s">
-        <v>103</v>
-      </c>
-      <c r="B18" s="26">
-        <v>18</v>
+        <v>120</v>
+      </c>
+      <c r="B18" s="26" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="14" t="s">
-        <v>104</v>
-      </c>
-      <c r="B19" s="26">
-        <v>19</v>
+        <v>122</v>
+      </c>
+      <c r="B19" s="26" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="14" t="s">
-        <v>105</v>
-      </c>
-      <c r="B20" s="26">
-        <v>20</v>
+        <v>124</v>
+      </c>
+      <c r="B20" s="26" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="B21" s="26">
-        <v>21</v>
+        <v>126</v>
+      </c>
+      <c r="B21" s="26" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>107</v>
+        <v>128</v>
       </c>
       <c r="B22" s="26">
         <v>22</v>
@@ -1704,7 +1775,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
@@ -1780,7 +1851,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2082,7 +2153,7 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2236,7 +2307,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E7 E8:E1048576" xr:uid="{00000000-0002-0000-0D00-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E7 E8:E1048576">
       <formula1>"Число, Диапазон, Логический"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2246,7 +2317,7 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
@@ -2309,7 +2380,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>116</v>
+        <v>137</v>
       </c>
       <c r="B7" s="11">
         <v>8</v>
@@ -2320,8 +2391,47 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="64" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>165</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2340,8 +2450,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="36" t="s">
-        <v>115</v>
+      <c r="A1" s="54" t="s">
+        <v>136</v>
       </c>
       <c r="B1" s="51" t="s">
         <v>8</v>
@@ -2349,24 +2459,24 @@
       <c r="C1" s="51" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="60" t="s">
+      <c r="D1" s="61" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="61" t="s">
+      <c r="E1" s="62" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="59" t="s">
+      <c r="F1" s="60" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="59"/>
-      <c r="H1" s="59"/>
+      <c r="G1" s="60"/>
+      <c r="H1" s="60"/>
     </row>
     <row r="2" spans="1:8" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="36"/>
+      <c r="A2" s="54"/>
       <c r="B2" s="51"/>
       <c r="C2" s="51"/>
-      <c r="D2" s="60"/>
-      <c r="E2" s="62"/>
+      <c r="D2" s="61"/>
+      <c r="E2" s="63"/>
       <c r="F2" s="27" t="s">
         <v>13</v>
       </c>
@@ -2387,13 +2497,13 @@
     <mergeCell ref="E1:E2"/>
   </mergeCells>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A3:A1048576" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A3:A1048576">
       <formula1>Код_ДР</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:B1048576" xr:uid="{00000000-0002-0000-0100-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:B1048576">
       <formula1>Вид_КУ</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C1048576" xr:uid="{00000000-0002-0000-0100-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C1048576">
       <formula1>INDIRECT(SUBSTITUTE($B3," ","_"))</formula1>
     </dataValidation>
   </dataValidations>
@@ -2403,12 +2513,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:P1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N1"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H2" sqref="H2"/>
+      <selection pane="bottomLeft" activeCell="H999" sqref="H999"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2420,70 +2530,56 @@
     <col min="5" max="5" width="22.7109375" style="5" customWidth="1"/>
     <col min="6" max="9" width="21.85546875" style="5" customWidth="1"/>
     <col min="10" max="10" width="21.85546875" style="35" customWidth="1"/>
-    <col min="11" max="11" width="30.85546875" style="5" customWidth="1"/>
-    <col min="12" max="12" width="37.7109375" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="23" t="s">
-        <v>115</v>
+        <v>136</v>
       </c>
       <c r="B1" s="31" t="s">
-        <v>121</v>
+        <v>142</v>
       </c>
       <c r="C1" s="24" t="s">
         <v>15</v>
       </c>
       <c r="D1" s="23" t="s">
-        <v>136</v>
+        <v>156</v>
       </c>
       <c r="E1" s="30" t="s">
-        <v>117</v>
+        <v>138</v>
       </c>
       <c r="F1" s="27" t="s">
         <v>16</v>
       </c>
       <c r="G1" s="30" t="s">
-        <v>139</v>
+        <v>159</v>
       </c>
       <c r="H1" s="34" t="s">
-        <v>140</v>
+        <v>160</v>
       </c>
       <c r="I1" s="30" t="s">
-        <v>141</v>
+        <v>161</v>
       </c>
       <c r="J1" s="34" t="s">
-        <v>142</v>
-      </c>
-      <c r="K1" s="30" t="s">
-        <v>135</v>
-      </c>
-      <c r="L1" s="30" t="s">
-        <v>126</v>
-      </c>
+        <v>162</v>
+      </c>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
       <c r="M1" s="2"/>
       <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
     </row>
   </sheetData>
-  <dataValidations count="6">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A1048576" xr:uid="{00000000-0002-0000-0200-000000000000}">
+  <dataValidations count="4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A1048576">
       <formula1>Код_ДР</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B1048576" xr:uid="{00000000-0002-0000-0200-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B1048576">
       <formula1>Тип_дома</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K1048576" xr:uid="{00000000-0002-0000-0200-000002000000}">
-      <formula1>"РСО, Исполнитель коммунальных услуг"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L1048576" xr:uid="{00000000-0002-0000-0200-000003000000}">
-      <formula1>"Да, Нет"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2" xr:uid="{64E806E2-203E-4524-A155-8726B23A3F98}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G1000">
       <formula1>"Нежилое помещение,Отдельная квартира,Коммунальная квартира,Общежитие"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2" xr:uid="{EA8A1693-1F91-404C-B6F7-A14618478727}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H1001">
       <formula1>"Да,Нет"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2493,7 +2589,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2515,44 +2611,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="36" t="s">
-        <v>115</v>
-      </c>
-      <c r="B1" s="36" t="s">
+      <c r="A1" s="54" t="s">
+        <v>136</v>
+      </c>
+      <c r="B1" s="54" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="59" t="s">
-        <v>120</v>
-      </c>
-      <c r="D1" s="49" t="s">
+      <c r="C1" s="60" t="s">
+        <v>141</v>
+      </c>
+      <c r="D1" s="39" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="41" t="s">
+      <c r="E1" s="52" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="41" t="s">
+      <c r="F1" s="52" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="60" t="s">
+      <c r="G1" s="61" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="61" t="s">
+      <c r="H1" s="62" t="s">
         <v>11</v>
       </c>
-      <c r="I1" s="62" t="s">
+      <c r="I1" s="63" t="s">
         <v>81</v>
       </c>
-      <c r="J1" s="62"/>
+      <c r="J1" s="63"/>
     </row>
     <row r="2" spans="1:10" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="36"/>
-      <c r="B2" s="36"/>
-      <c r="C2" s="49"/>
-      <c r="D2" s="49"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="60"/>
-      <c r="H2" s="62"/>
+      <c r="A2" s="54"/>
+      <c r="B2" s="54"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
+      <c r="G2" s="61"/>
+      <c r="H2" s="63"/>
       <c r="I2" s="28" t="s">
         <v>82</v>
       </c>
@@ -2578,28 +2674,28 @@
     <mergeCell ref="F1:F2"/>
   </mergeCells>
   <dataValidations count="8">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A3:A1048576" xr:uid="{00000000-0002-0000-0300-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A3:A1048576">
       <formula1>Код_ДР</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:B1048576" xr:uid="{00000000-0002-0000-0300-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:B1048576">
       <formula1>Адрес_ОЖФ</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C1048576" xr:uid="{00000000-0002-0000-0300-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C1048576">
       <formula1>Номер_квартиры</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3:D1048576" xr:uid="{00000000-0002-0000-0300-000003000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3:D1048576">
       <formula1>Номер_комнаты</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E1048576" xr:uid="{00000000-0002-0000-0300-000004000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E1048576">
       <formula1>Вид_КУ</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F1048576" xr:uid="{00000000-0002-0000-0300-000005000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F1048576">
       <formula1>INDIRECT(SUBSTITUTE($E3," ","_"))</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I3:I1048576" xr:uid="{00000000-0002-0000-0300-000006000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I3:I1048576">
       <formula1>"Открытая, Закрытая"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J3:J1048576" xr:uid="{00000000-0002-0000-0300-000007000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J3:J1048576">
       <formula1>"Централизованная, Нецентрализованная"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2608,12 +2704,12 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="4" topLeftCell="E1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="N1" sqref="N1:N1048576"/>
+      <selection pane="topRight" activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2635,13 +2731,13 @@
   <sheetData>
     <row r="1" spans="1:13" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="23" t="s">
-        <v>115</v>
+        <v>136</v>
       </c>
       <c r="B1" s="27" t="s">
         <v>15</v>
       </c>
       <c r="C1" s="30" t="s">
-        <v>120</v>
+        <v>141</v>
       </c>
       <c r="D1" s="27" t="s">
         <v>16</v>
@@ -2671,34 +2767,34 @@
         <v>54</v>
       </c>
       <c r="M1" s="32" t="s">
-        <v>133</v>
+        <v>154</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="9">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A1048576" xr:uid="{00000000-0002-0000-0400-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A1048576">
       <formula1>Код_ДР</formula1>
     </dataValidation>
-    <dataValidation operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1 E1:M1" xr:uid="{00000000-0002-0000-0400-000001000000}"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576" xr:uid="{00000000-0002-0000-0400-000002000000}">
+    <dataValidation operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1 E1:M1"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576">
       <formula1>Номер_комнаты</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C1048576" xr:uid="{00000000-0002-0000-0400-000003000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C1048576">
       <formula1>Номер_квартиры</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B1048576" xr:uid="{00000000-0002-0000-0400-000004000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B1048576">
       <formula1>Адрес_ОЖФ</formula1>
     </dataValidation>
-    <dataValidation type="list" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K1048576" xr:uid="{00000000-0002-0000-0400-000005000000}">
+    <dataValidation type="list" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K1048576">
       <formula1>"Соответствует, Не соответствует"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G1048576" xr:uid="{00000000-0002-0000-0400-000006000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G1048576">
       <formula1>INDIRECT(SUBSTITUTE(CONCATENATE(E2," ",F2)," ","_"))</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F1048576" xr:uid="{00000000-0002-0000-0400-000007000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F1048576">
       <formula1>INDIRECT(SUBSTITUTE($E2," ","_"))</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E1048576" xr:uid="{00000000-0002-0000-0400-000008000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E1048576">
       <formula1>Вид_КУ</formula1>
     </dataValidation>
   </dataValidations>
@@ -2708,12 +2804,12 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:M1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="4" topLeftCell="N1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="N1" sqref="N1:N1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="4" topLeftCell="E1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2725,22 +2821,23 @@
     <col min="5" max="5" width="21.5703125" customWidth="1"/>
     <col min="6" max="6" width="22" customWidth="1"/>
     <col min="7" max="7" width="29.5703125" style="5" customWidth="1"/>
-    <col min="8" max="9" width="27.5703125" style="5" customWidth="1"/>
-    <col min="10" max="10" width="25" style="5" customWidth="1"/>
-    <col min="11" max="11" width="27.5703125" style="5" customWidth="1"/>
-    <col min="12" max="12" width="17.5703125" style="5" customWidth="1"/>
-    <col min="13" max="13" width="33.7109375" style="5" customWidth="1"/>
+    <col min="8" max="8" width="29.5703125" customWidth="1"/>
+    <col min="9" max="10" width="27.5703125" style="5" customWidth="1"/>
+    <col min="11" max="11" width="25" style="5" customWidth="1"/>
+    <col min="12" max="12" width="27.5703125" style="5" customWidth="1"/>
+    <col min="13" max="13" width="17.5703125" style="5" customWidth="1"/>
+    <col min="14" max="14" width="33.7109375" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="23" t="s">
-        <v>115</v>
+        <v>136</v>
       </c>
       <c r="B1" s="27" t="s">
         <v>15</v>
       </c>
       <c r="C1" s="30" t="s">
-        <v>120</v>
+        <v>141</v>
       </c>
       <c r="D1" s="27" t="s">
         <v>16</v>
@@ -2754,61 +2851,76 @@
       <c r="G1" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="27" t="s">
+      <c r="H1" s="36" t="s">
+        <v>166</v>
+      </c>
+      <c r="I1" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="I1" s="27" t="s">
+      <c r="J1" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="J1" s="27" t="s">
+      <c r="K1" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="K1" s="27" t="s">
+      <c r="L1" s="27" t="s">
         <v>84</v>
       </c>
-      <c r="L1" s="27" t="s">
+      <c r="M1" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="M1" s="32" t="s">
-        <v>133</v>
+      <c r="N1" s="32" t="s">
+        <v>154</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="8">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A1048576" xr:uid="{00000000-0002-0000-0500-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A1048576">
       <formula1>Код_ДР</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576" xr:uid="{00000000-0002-0000-0500-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576">
       <formula1>Номер_комнаты</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C1048576" xr:uid="{00000000-0002-0000-0500-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C1048576">
       <formula1>Номер_квартиры</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B1048576" xr:uid="{00000000-0002-0000-0500-000003000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B1048576">
       <formula1>Адрес_ОЖФ</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F1048576" xr:uid="{00000000-0002-0000-0500-000004000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F1048576">
       <formula1>INDIRECT(SUBSTITUTE($E2," ","_"))</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E1048576" xr:uid="{00000000-0002-0000-0500-000005000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E1048576">
       <formula1>Вид_КУ</formula1>
     </dataValidation>
-    <dataValidation operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H1:J1048576 K1" xr:uid="{00000000-0002-0000-0500-000006000000}"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K1048576" xr:uid="{00000000-0002-0000-0500-000007000000}">
+    <dataValidation operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I1:K1048576 L1"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L1048576">
       <formula1>"Соответствует, Не соответствует"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>'Тип Поля'!$A$2:$A$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>H2:H1000</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2825,22 +2937,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="36" t="s">
-        <v>115</v>
-      </c>
-      <c r="B1" s="36" t="s">
+      <c r="A1" s="54" t="s">
+        <v>136</v>
+      </c>
+      <c r="B1" s="54" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="59" t="s">
-        <v>128</v>
-      </c>
-      <c r="D1" s="49" t="s">
+      <c r="C1" s="60" t="s">
+        <v>149</v>
+      </c>
+      <c r="D1" s="39" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="41" t="s">
+      <c r="E1" s="52" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="41" t="s">
+      <c r="F1" s="52" t="s">
         <v>9</v>
       </c>
       <c r="G1" s="51" t="s">
@@ -2850,12 +2962,12 @@
       <c r="I1" s="51"/>
     </row>
     <row r="2" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="36"/>
-      <c r="B2" s="36"/>
-      <c r="C2" s="49"/>
-      <c r="D2" s="49"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
+      <c r="A2" s="54"/>
+      <c r="B2" s="54"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
       <c r="G2" s="33" t="s">
         <v>13</v>
       </c>
@@ -2877,22 +2989,22 @@
     <mergeCell ref="F1:F2"/>
   </mergeCells>
   <dataValidations count="6">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F1048576" xr:uid="{00000000-0002-0000-0600-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F1048576">
       <formula1>INDIRECT(SUBSTITUTE($E3," ","_"))</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E1048576" xr:uid="{00000000-0002-0000-0600-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E1048576">
       <formula1>Вид_КУ</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A3:A1048576" xr:uid="{00000000-0002-0000-0600-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A3:A1048576">
       <formula1>Код_ДР</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3:D1048576" xr:uid="{00000000-0002-0000-0600-000003000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3:D1048576">
       <formula1>Номер_комнаты</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C1048576" xr:uid="{00000000-0002-0000-0600-000004000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C1048576">
       <formula1>Номер_квартиры</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:B1048576" xr:uid="{00000000-0002-0000-0600-000005000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:B1048576">
       <formula1>Адрес_ОЖФ</formula1>
     </dataValidation>
   </dataValidations>
@@ -2901,12 +3013,12 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="4" topLeftCell="E1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H1" sqref="H1:H1048576"/>
+      <selection pane="topRight" activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2922,13 +3034,13 @@
   <sheetData>
     <row r="1" spans="1:7" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="23" t="s">
-        <v>115</v>
+        <v>136</v>
       </c>
       <c r="B1" s="27" t="s">
         <v>15</v>
       </c>
       <c r="C1" s="30" t="s">
-        <v>120</v>
+        <v>141</v>
       </c>
       <c r="D1" s="27" t="s">
         <v>16</v>
@@ -2945,17 +3057,17 @@
     </row>
   </sheetData>
   <dataValidations count="5">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A1048576" xr:uid="{00000000-0002-0000-0700-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A1048576">
       <formula1>Код_ДР</formula1>
     </dataValidation>
-    <dataValidation operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:G1 F2:G1048576" xr:uid="{00000000-0002-0000-0700-000001000000}"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B1048576" xr:uid="{00000000-0002-0000-0700-000003000000}">
+    <dataValidation operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:G1 F2:G1048576"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B1048576">
       <formula1>Адрес_ОЖФ</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C1048576" xr:uid="{00000000-0002-0000-0700-000004000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C1048576">
       <formula1>Номер_квартиры</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576" xr:uid="{00000000-0002-0000-0700-000005000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576">
       <formula1>Номер_комнаты</formula1>
     </dataValidation>
   </dataValidations>
@@ -2965,7 +3077,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2977,17 +3089,17 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>122</v>
+        <v>143</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>123</v>
+        <v>144</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>124</v>
+        <v>145</v>
       </c>
     </row>
   </sheetData>

</xml_diff>